<commit_message>
Finishes metrics html display
</commit_message>
<xml_diff>
--- a/spec/support/fixtures/contracts.xlsx
+++ b/spec/support/fixtures/contracts.xlsx
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:AF1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,22 +549,22 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>41699</v>
+        <v>41548</v>
       </c>
       <c r="C2" s="1">
-        <v>42063</v>
+        <v>41912</v>
       </c>
       <c r="D2">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
-        <v>60000</v>
+        <v>3000</v>
       </c>
       <c r="F2" s="1">
-        <v>41306</v>
+        <v>41547</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -573,13 +573,13 @@
         <v>12</v>
       </c>
       <c r="I2" s="2">
-        <v>2500</v>
+        <v>250</v>
       </c>
       <c r="J2" s="2">
-        <v>30000</v>
+        <v>3000</v>
       </c>
       <c r="K2" s="3">
-        <v>30000</v>
+        <v>1000</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -587,22 +587,22 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
-        <v>42064</v>
+        <v>41548</v>
       </c>
       <c r="C3" s="1">
-        <v>42429</v>
+        <v>41912</v>
       </c>
       <c r="D3">
         <v>12</v>
       </c>
       <c r="E3" s="2">
-        <v>33000</v>
+        <v>2388</v>
       </c>
       <c r="F3" s="1">
-        <v>41944</v>
+        <v>41547</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -611,13 +611,13 @@
         <v>12</v>
       </c>
       <c r="I3" s="2">
-        <v>2750</v>
+        <v>199</v>
       </c>
       <c r="J3" s="2">
-        <v>33000</v>
-      </c>
-      <c r="K3" s="3">
-        <v>30000</v>
+        <v>2388</v>
+      </c>
+      <c r="K3">
+        <v>300</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -625,7 +625,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>41699</v>
@@ -634,13 +634,13 @@
         <v>42063</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2">
-        <v>4200</v>
+        <v>60000</v>
       </c>
       <c r="F4" s="1">
-        <v>41699</v>
+        <v>41306</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -649,13 +649,13 @@
         <v>12</v>
       </c>
       <c r="I4" s="2">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="J4" s="2">
-        <v>4200</v>
-      </c>
-      <c r="K4">
-        <v>300</v>
+        <v>30000</v>
+      </c>
+      <c r="K4" s="3">
+        <v>30000</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -663,57 +663,57 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>41883</v>
+        <v>41699</v>
       </c>
       <c r="C5" s="1">
-        <v>42429</v>
+        <v>42063</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2">
-        <v>567</v>
+        <v>4200</v>
       </c>
       <c r="F5" s="1">
-        <v>42035</v>
+        <v>41699</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="2">
-        <v>567</v>
+        <v>350</v>
       </c>
       <c r="J5" s="2">
-        <v>6804</v>
+        <v>4200</v>
       </c>
       <c r="K5">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1">
-        <v>41912</v>
+        <v>41820</v>
       </c>
       <c r="C6" s="1">
-        <v>42276</v>
+        <v>42184</v>
       </c>
       <c r="D6">
         <v>12</v>
       </c>
       <c r="E6" s="2">
-        <v>1188</v>
+        <v>2004</v>
       </c>
       <c r="F6" s="1">
-        <v>41912</v>
+        <v>41820</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -722,68 +722,68 @@
         <v>12</v>
       </c>
       <c r="I6" s="2">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="J6" s="2">
-        <v>1188</v>
-      </c>
-      <c r="K6">
-        <v>100</v>
+        <v>2004</v>
+      </c>
+      <c r="K6" s="3">
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>41913</v>
+        <v>41883</v>
       </c>
       <c r="C7" s="1">
-        <v>42277</v>
+        <v>42429</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>3000</v>
+        <v>567</v>
       </c>
       <c r="F7" s="1">
-        <v>42277</v>
+        <v>42035</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="2">
-        <v>250</v>
+        <v>567</v>
       </c>
       <c r="J7" s="2">
-        <v>3000</v>
-      </c>
-      <c r="K7" s="3">
-        <v>1000</v>
+        <v>6804</v>
+      </c>
+      <c r="K7">
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>41548</v>
+        <v>41912</v>
       </c>
       <c r="C8" s="1">
-        <v>41912</v>
+        <v>42276</v>
       </c>
       <c r="D8">
         <v>12</v>
       </c>
       <c r="E8" s="2">
-        <v>3000</v>
+        <v>1188</v>
       </c>
       <c r="F8" s="1">
-        <v>41547</v>
+        <v>41912</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -792,18 +792,18 @@
         <v>12</v>
       </c>
       <c r="I8" s="2">
-        <v>250</v>
+        <v>99</v>
       </c>
       <c r="J8" s="2">
-        <v>3000</v>
-      </c>
-      <c r="K8" s="3">
-        <v>1000</v>
+        <v>1188</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>41913</v>
@@ -815,10 +815,10 @@
         <v>12</v>
       </c>
       <c r="E9" s="2">
-        <v>2388</v>
+        <v>3000</v>
       </c>
       <c r="F9" s="1">
-        <v>41912</v>
+        <v>42277</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -827,13 +827,13 @@
         <v>12</v>
       </c>
       <c r="I9" s="2">
-        <v>199</v>
+        <v>250</v>
       </c>
       <c r="J9" s="2">
-        <v>2388</v>
-      </c>
-      <c r="K9">
-        <v>300</v>
+        <v>3000</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -841,10 +841,10 @@
         <v>18</v>
       </c>
       <c r="B10" s="1">
-        <v>41548</v>
+        <v>41913</v>
       </c>
       <c r="C10" s="1">
-        <v>41912</v>
+        <v>42277</v>
       </c>
       <c r="D10">
         <v>12</v>
@@ -853,7 +853,7 @@
         <v>2388</v>
       </c>
       <c r="F10" s="1">
-        <v>41547</v>
+        <v>41912</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -873,77 +873,77 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1">
-        <v>41974</v>
+        <v>41944</v>
       </c>
       <c r="C11" s="1">
-        <v>42338</v>
+        <v>42035</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E11" s="2">
-        <v>2438</v>
+        <v>2001</v>
       </c>
       <c r="F11" s="1">
-        <v>42338</v>
+        <v>41944</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I11" s="2">
-        <v>203.16666666666666</v>
+        <v>667</v>
       </c>
       <c r="J11" s="2">
-        <v>2438</v>
-      </c>
-      <c r="K11">
-        <v>650</v>
+        <v>8004</v>
+      </c>
+      <c r="K11" s="3">
+        <v>800</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
-        <v>42005</v>
+        <v>41974</v>
       </c>
       <c r="C12" s="1">
-        <v>42369</v>
+        <v>42338</v>
       </c>
       <c r="D12">
         <v>12</v>
       </c>
       <c r="E12" s="2">
-        <v>198000</v>
+        <v>2438</v>
       </c>
       <c r="F12" s="1">
-        <v>41944</v>
+        <v>42338</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I12" s="2">
-        <v>16500</v>
+        <v>203.16666666666666</v>
       </c>
       <c r="J12" s="2">
-        <v>198000</v>
-      </c>
-      <c r="K12" s="3">
-        <v>5000</v>
+        <v>2438</v>
+      </c>
+      <c r="K12">
+        <v>650</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>42005</v>
@@ -955,30 +955,30 @@
         <v>12</v>
       </c>
       <c r="E13" s="2">
-        <v>9910</v>
+        <v>198000</v>
       </c>
       <c r="F13" s="1">
-        <v>42004</v>
+        <v>41944</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="I13" s="2">
-        <v>825.83333333333337</v>
+        <v>16500</v>
       </c>
       <c r="J13" s="2">
-        <v>9910</v>
-      </c>
-      <c r="K13">
-        <v>750</v>
+        <v>198000</v>
+      </c>
+      <c r="K13" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
         <v>42005</v>
@@ -990,10 +990,10 @@
         <v>12</v>
       </c>
       <c r="E14" s="2">
-        <v>1200</v>
+        <v>9910</v>
       </c>
       <c r="F14" s="1">
-        <v>42369</v>
+        <v>42004</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -1002,18 +1002,18 @@
         <v>12</v>
       </c>
       <c r="I14" s="2">
-        <v>100</v>
+        <v>825.83333333333337</v>
       </c>
       <c r="J14" s="2">
-        <v>1200</v>
+        <v>9910</v>
       </c>
       <c r="K14">
-        <v>100</v>
+        <v>750</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
         <v>42005</v>
@@ -1025,45 +1025,45 @@
         <v>12</v>
       </c>
       <c r="E15" s="2">
-        <v>8640</v>
+        <v>1200</v>
       </c>
       <c r="F15" s="1">
-        <v>42094</v>
+        <v>42369</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I15" s="2">
-        <v>720</v>
+        <v>100</v>
       </c>
       <c r="J15" s="2">
-        <v>8640</v>
-      </c>
-      <c r="K15" s="3">
-        <v>2000</v>
+        <v>1200</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1">
-        <v>42036</v>
+        <v>42005</v>
       </c>
       <c r="C16" s="1">
-        <v>42400</v>
+        <v>42369</v>
       </c>
       <c r="D16">
         <v>12</v>
       </c>
       <c r="E16" s="2">
-        <v>19000</v>
+        <v>8640</v>
       </c>
       <c r="F16" s="1">
-        <v>42063</v>
+        <v>42094</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -1072,53 +1072,53 @@
         <v>25</v>
       </c>
       <c r="I16" s="2">
-        <v>1583.3333333333333</v>
+        <v>720</v>
       </c>
       <c r="J16" s="2">
-        <v>19000</v>
+        <v>8640</v>
       </c>
       <c r="K16" s="3">
-        <v>20000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1">
-        <v>42064</v>
+        <v>42036</v>
       </c>
       <c r="C17" s="1">
-        <v>42429</v>
+        <v>42400</v>
       </c>
       <c r="D17">
         <v>12</v>
       </c>
       <c r="E17" s="2">
-        <v>4200</v>
+        <v>19000</v>
       </c>
       <c r="F17" s="1">
-        <v>42094</v>
+        <v>42063</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I17" s="2">
-        <v>350</v>
+        <v>1583.3333333333333</v>
       </c>
       <c r="J17" s="2">
-        <v>4200</v>
-      </c>
-      <c r="K17">
-        <v>300</v>
+        <v>19000</v>
+      </c>
+      <c r="K17" s="3">
+        <v>20000</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1">
         <v>42064</v>
@@ -1130,10 +1130,10 @@
         <v>12</v>
       </c>
       <c r="E18" s="2">
-        <v>45000</v>
+        <v>33000</v>
       </c>
       <c r="F18" s="1">
-        <v>42094</v>
+        <v>41944</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
@@ -1142,30 +1142,30 @@
         <v>12</v>
       </c>
       <c r="I18" s="2">
-        <v>3750</v>
+        <v>2750</v>
       </c>
       <c r="J18" s="2">
-        <v>45000</v>
+        <v>33000</v>
       </c>
       <c r="K18" s="3">
-        <v>10000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1">
-        <v>42095</v>
+        <v>42064</v>
       </c>
       <c r="C19" s="1">
-        <v>42460</v>
+        <v>42429</v>
       </c>
       <c r="D19">
         <v>12</v>
       </c>
       <c r="E19" s="2">
-        <v>1650</v>
+        <v>4200</v>
       </c>
       <c r="F19" s="1">
         <v>42094</v>
@@ -1177,30 +1177,30 @@
         <v>12</v>
       </c>
       <c r="I19" s="2">
-        <v>137.5</v>
+        <v>350</v>
       </c>
       <c r="J19" s="2">
-        <v>1650</v>
+        <v>4200</v>
       </c>
       <c r="K19">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1">
-        <v>42095</v>
+        <v>42064</v>
       </c>
       <c r="C20" s="1">
-        <v>42460</v>
+        <v>42429</v>
       </c>
       <c r="D20">
         <v>12</v>
       </c>
       <c r="E20" s="2">
-        <v>900</v>
+        <v>45000</v>
       </c>
       <c r="F20" s="1">
         <v>42094</v>
@@ -1209,36 +1209,36 @@
         <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I20" s="2">
-        <v>75</v>
+        <v>3750</v>
       </c>
       <c r="J20" s="2">
-        <v>900</v>
-      </c>
-      <c r="K20">
-        <v>200</v>
+        <v>45000</v>
+      </c>
+      <c r="K20" s="3">
+        <v>10000</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1">
-        <v>42103</v>
+        <v>42095</v>
       </c>
       <c r="C21" s="1">
-        <v>42468</v>
+        <v>42460</v>
       </c>
       <c r="D21">
         <v>12</v>
       </c>
       <c r="E21" s="2">
-        <v>2700</v>
+        <v>1650</v>
       </c>
       <c r="F21" s="1">
-        <v>42124</v>
+        <v>42094</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
@@ -1247,10 +1247,10 @@
         <v>12</v>
       </c>
       <c r="I21" s="2">
-        <v>225</v>
+        <v>137.5</v>
       </c>
       <c r="J21" s="2">
-        <v>2700</v>
+        <v>1650</v>
       </c>
       <c r="K21">
         <v>200</v>
@@ -1258,34 +1258,34 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1">
-        <v>42177</v>
+        <v>42095</v>
       </c>
       <c r="C22" s="1">
-        <v>42542</v>
+        <v>42460</v>
       </c>
       <c r="D22">
         <v>12</v>
       </c>
       <c r="E22" s="2">
-        <v>2700</v>
+        <v>900</v>
       </c>
       <c r="F22" s="1">
-        <v>42177</v>
+        <v>42094</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I22" s="2">
-        <v>225</v>
+        <v>75</v>
       </c>
       <c r="J22" s="2">
-        <v>2700</v>
+        <v>900</v>
       </c>
       <c r="K22">
         <v>200</v>
@@ -1293,22 +1293,22 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1">
-        <v>42186</v>
+        <v>42103</v>
       </c>
       <c r="C23" s="1">
-        <v>42551</v>
+        <v>42468</v>
       </c>
       <c r="D23">
         <v>12</v>
       </c>
       <c r="E23" s="2">
-        <v>3600</v>
+        <v>2700</v>
       </c>
       <c r="F23" s="1">
-        <v>42186</v>
+        <v>42124</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
@@ -1317,243 +1317,243 @@
         <v>12</v>
       </c>
       <c r="I23" s="2">
-        <v>300</v>
+        <v>225</v>
       </c>
       <c r="J23" s="2">
-        <v>3600</v>
+        <v>2700</v>
       </c>
       <c r="K23">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1">
-        <v>42217</v>
+        <v>42142</v>
       </c>
       <c r="C24" s="1">
-        <v>42400</v>
+        <v>42202</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2">
-        <v>36000</v>
+        <v>82</v>
       </c>
       <c r="F24" s="1">
-        <v>42217</v>
+        <v>42125</v>
       </c>
       <c r="G24" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="H24" t="s">
         <v>12</v>
       </c>
       <c r="I24" s="2">
-        <v>6000</v>
+        <v>82</v>
       </c>
       <c r="J24" s="2">
-        <v>72000</v>
+        <v>984</v>
       </c>
       <c r="K24" s="3">
-        <v>75000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1">
-        <v>42224</v>
+        <v>42177</v>
       </c>
       <c r="C25" s="1">
-        <v>42436</v>
+        <v>42542</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E25" s="2">
-        <v>200</v>
+        <v>2700</v>
       </c>
       <c r="F25" s="1">
-        <v>42224</v>
+        <v>42177</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H25" t="s">
         <v>12</v>
       </c>
       <c r="I25" s="2">
-        <v>300</v>
+        <v>225</v>
       </c>
       <c r="J25" s="2">
-        <v>3600</v>
+        <v>2700</v>
       </c>
       <c r="K25">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1">
-        <v>42227</v>
+        <v>42186</v>
       </c>
       <c r="C26" s="1">
-        <v>42592</v>
+        <v>42551</v>
       </c>
       <c r="D26">
         <v>12</v>
       </c>
       <c r="E26" s="2">
-        <v>9750</v>
+        <v>3600</v>
       </c>
       <c r="F26" s="1">
-        <v>42227</v>
+        <v>42186</v>
       </c>
       <c r="G26" t="s">
         <v>11</v>
       </c>
       <c r="H26" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I26" s="2">
-        <v>812.5</v>
+        <v>300</v>
       </c>
       <c r="J26" s="2">
-        <v>9750</v>
-      </c>
-      <c r="K26" s="3">
-        <v>4000</v>
+        <v>3600</v>
+      </c>
+      <c r="K26">
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1">
-        <v>42231</v>
+        <v>42217</v>
       </c>
       <c r="C27" s="1">
-        <v>42596</v>
+        <v>42400</v>
       </c>
       <c r="D27">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E27" s="2">
-        <v>3330</v>
+        <v>36000</v>
       </c>
       <c r="F27" s="1">
-        <v>42231</v>
+        <v>42217</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
         <v>12</v>
       </c>
       <c r="I27" s="2">
-        <v>277.5</v>
+        <v>6000</v>
       </c>
       <c r="J27" s="2">
-        <v>3330</v>
-      </c>
-      <c r="K27">
-        <v>313</v>
+        <v>72000</v>
+      </c>
+      <c r="K27" s="3">
+        <v>75000</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1">
-        <v>42248</v>
+        <v>42224</v>
       </c>
       <c r="C28" s="1">
-        <v>42613</v>
+        <v>42436</v>
       </c>
       <c r="D28">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2">
-        <v>1250</v>
+        <v>200</v>
       </c>
       <c r="F28" s="1">
-        <v>42248</v>
+        <v>42224</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H28" t="s">
         <v>12</v>
       </c>
       <c r="I28" s="2">
-        <v>104.16666666666667</v>
+        <v>300</v>
       </c>
       <c r="J28" s="2">
-        <v>1250</v>
+        <v>3600</v>
       </c>
       <c r="K28">
-        <v>250</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1">
-        <v>42256</v>
+        <v>42227</v>
       </c>
       <c r="C29" s="1">
-        <v>42437</v>
+        <v>42592</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E29" s="2">
-        <v>60</v>
+        <v>9750</v>
       </c>
       <c r="F29" s="1">
-        <v>42256</v>
+        <v>42227</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H29" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I29" s="2">
-        <v>60</v>
+        <v>812.5</v>
       </c>
       <c r="J29" s="2">
-        <v>720</v>
-      </c>
-      <c r="K29">
-        <v>60</v>
+        <v>9750</v>
+      </c>
+      <c r="K29" s="3">
+        <v>4000</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>42258</v>
+        <v>42231</v>
       </c>
       <c r="C30" s="1">
-        <v>42623</v>
+        <v>42596</v>
       </c>
       <c r="D30">
         <v>12</v>
       </c>
       <c r="E30" s="2">
-        <v>500</v>
+        <v>3330</v>
       </c>
       <c r="F30" s="1">
-        <v>42258</v>
+        <v>42231</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
@@ -1562,68 +1562,68 @@
         <v>12</v>
       </c>
       <c r="I30" s="2">
-        <v>41.666666666666664</v>
+        <v>277.5</v>
       </c>
       <c r="J30" s="2">
-        <v>500</v>
+        <v>3330</v>
       </c>
       <c r="K30">
-        <v>50</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1">
-        <v>42265</v>
+        <v>42248</v>
       </c>
       <c r="C31" s="1">
-        <v>42446</v>
+        <v>42613</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E31" s="2">
-        <v>50</v>
+        <v>1250</v>
       </c>
       <c r="F31" s="1">
-        <v>42265</v>
+        <v>42248</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="2">
-        <v>50</v>
+        <v>104.16666666666667</v>
       </c>
       <c r="J31" s="2">
-        <v>600</v>
+        <v>1250</v>
       </c>
       <c r="K31">
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1">
-        <v>42274</v>
+        <v>42256</v>
       </c>
       <c r="C32" s="1">
-        <v>42426</v>
+        <v>42437</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" s="2">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="F32" s="1">
-        <v>42274</v>
+        <v>42256</v>
       </c>
       <c r="G32" t="s">
         <v>15</v>
@@ -1632,33 +1632,33 @@
         <v>12</v>
       </c>
       <c r="I32" s="2">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="J32" s="2">
-        <v>1296</v>
+        <v>720</v>
       </c>
       <c r="K32">
-        <v>108</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1">
-        <v>42277</v>
+        <v>42258</v>
       </c>
       <c r="C33" s="1">
-        <v>42642</v>
+        <v>42623</v>
       </c>
       <c r="D33">
         <v>12</v>
       </c>
       <c r="E33" s="2">
-        <v>1188</v>
+        <v>500</v>
       </c>
       <c r="F33" s="1">
-        <v>42277</v>
+        <v>42258</v>
       </c>
       <c r="G33" t="s">
         <v>11</v>
@@ -1667,103 +1667,103 @@
         <v>12</v>
       </c>
       <c r="I33" s="2">
-        <v>49.5</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="J33" s="2">
-        <v>594</v>
+        <v>500</v>
       </c>
       <c r="K33">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1">
-        <v>42278</v>
+        <v>42265</v>
       </c>
       <c r="C34" s="1">
-        <v>42643</v>
+        <v>42446</v>
       </c>
       <c r="D34">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E34" s="2">
-        <v>3000</v>
+        <v>50</v>
       </c>
       <c r="F34" s="1">
-        <v>42278</v>
+        <v>42265</v>
       </c>
       <c r="G34" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H34" t="s">
         <v>12</v>
       </c>
       <c r="I34" s="2">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="J34" s="2">
-        <v>3000</v>
-      </c>
-      <c r="K34" s="3">
-        <v>1000</v>
+        <v>600</v>
+      </c>
+      <c r="K34">
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1">
-        <v>42278</v>
+        <v>42274</v>
       </c>
       <c r="C35" s="1">
-        <v>42643</v>
+        <v>42426</v>
       </c>
       <c r="D35">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E35" s="2">
-        <v>2388</v>
+        <v>108</v>
       </c>
       <c r="F35" s="1">
-        <v>42277</v>
+        <v>42274</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H35" t="s">
         <v>12</v>
       </c>
       <c r="I35" s="2">
-        <v>199</v>
+        <v>108</v>
       </c>
       <c r="J35" s="2">
-        <v>2388</v>
+        <v>1296</v>
       </c>
       <c r="K35">
-        <v>300</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B36" s="1">
-        <v>42278</v>
+        <v>42277</v>
       </c>
       <c r="C36" s="1">
-        <v>42643</v>
+        <v>42642</v>
       </c>
       <c r="D36">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" s="2">
-        <v>31500</v>
+        <v>1188</v>
       </c>
       <c r="F36" s="1">
-        <v>42278</v>
+        <v>42277</v>
       </c>
       <c r="G36" t="s">
         <v>11</v>
@@ -1772,33 +1772,33 @@
         <v>12</v>
       </c>
       <c r="I36" s="2">
-        <v>2423.0833333333335</v>
+        <v>49.5</v>
       </c>
       <c r="J36" s="2">
-        <v>29077</v>
-      </c>
-      <c r="K36" s="3">
-        <v>21000</v>
+        <v>594</v>
+      </c>
+      <c r="K36">
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="B37" s="1">
-        <v>41820</v>
+        <v>42278</v>
       </c>
       <c r="C37" s="1">
-        <v>42184</v>
+        <v>42643</v>
       </c>
       <c r="D37">
         <v>12</v>
       </c>
       <c r="E37" s="2">
-        <v>2004</v>
+        <v>3000</v>
       </c>
       <c r="F37" s="1">
-        <v>41820</v>
+        <v>42278</v>
       </c>
       <c r="G37" t="s">
         <v>11</v>
@@ -1807,83 +1807,83 @@
         <v>12</v>
       </c>
       <c r="I37" s="2">
-        <v>167</v>
+        <v>250</v>
       </c>
       <c r="J37" s="2">
-        <v>2004</v>
+        <v>3000</v>
       </c>
       <c r="K37" s="3">
-        <v>350</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B38" s="1">
-        <v>42142</v>
+        <v>42278</v>
       </c>
       <c r="C38" s="1">
-        <v>42202</v>
+        <v>42643</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E38" s="2">
-        <v>82</v>
+        <v>2388</v>
       </c>
       <c r="F38" s="1">
-        <v>42125</v>
+        <v>42277</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H38" t="s">
         <v>12</v>
       </c>
       <c r="I38" s="2">
-        <v>82</v>
+        <v>199</v>
       </c>
       <c r="J38" s="2">
-        <v>984</v>
-      </c>
-      <c r="K38" s="3">
-        <v>100</v>
+        <v>2388</v>
+      </c>
+      <c r="K38">
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1">
-        <v>41944</v>
+        <v>42278</v>
       </c>
       <c r="C39" s="1">
-        <v>42035</v>
+        <v>42643</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E39" s="2">
-        <v>2001</v>
+        <v>31500</v>
       </c>
       <c r="F39" s="1">
-        <v>41944</v>
+        <v>42278</v>
       </c>
       <c r="G39" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I39" s="2">
-        <v>667</v>
+        <v>2423.0833333333335</v>
       </c>
       <c r="J39" s="2">
-        <v>8004</v>
+        <v>29077</v>
       </c>
       <c r="K39" s="3">
-        <v>800</v>
+        <v>21000</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -8978,6 +8978,9 @@
       <c r="K1044" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="A2:K41">
+    <sortCondition ref="B2:B41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>